<commit_message>
changement couleur menu liens
</commit_message>
<xml_diff>
--- a/downloads/autorisation de prélèvement.xlsx
+++ b/downloads/autorisation de prélèvement.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>PPE</t>
   </si>
@@ -52,15 +52,6 @@
     <t xml:space="preserve">                                   …………………………………………………………………………………………………………………………………………………………………..</t>
   </si>
   <si>
-    <t>J'autorise l'Etablissement teneur de mon compte à effectuer sur ce dernier</t>
-  </si>
-  <si>
-    <t>ordonnés par le créancier désigné ci-dessous. En cas de litige sur un prélèvement, je pourrais en faire suspendre l'exécution</t>
-  </si>
-  <si>
-    <t>par simple demande à l'Etablissement teneur de mon compte. Je règlerai le différend directement avec le créancier.</t>
-  </si>
-  <si>
     <t>P.P.E</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
   </si>
   <si>
     <t>Signature</t>
-  </si>
-  <si>
-    <t>nier, si sa situation le permet, tous les prélèvements</t>
   </si>
   <si>
     <t>A retourner sous enveloppe à:</t>
@@ -120,12 +108,17 @@
     <t>Plus Forts Ensemble</t>
   </si>
   <si>
-    <t>La P.P.E a obtenu de la banque de France un Numéro National d'Emetteur pour un suivi des operations financières.
+    <t>N° National d'Emetteur</t>
+  </si>
+  <si>
+    <t>La P.P.E a obtenu de la banque de France un Numéro National d'Emetteur pour un suivi des opérations financières.
 Il suffit de remplir ce bordereau et de le retourner accompagné d'un relevé
 d'identité bancaire ou postal</t>
   </si>
   <si>
-    <t>N° National d'Emetteur</t>
+    <t>J'autorise l'Etablissement teneur de mon compte à effectuer sur ce dernier, si sa situation le permet, tous les prélèvements
+ordonnés par le créancier désigné ci‐dessous. En cas de litige sur un prélèvement, je pourrais en faire suspendre l'exécution
+par simple demande à l'Etablissement teneur de mon compte. Je règlerai le différend directement avec le créancier.</t>
   </si>
 </sst>
 </file>
@@ -547,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -669,6 +662,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1342,7 +1341,7 @@
   <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1354,9 +1353,8 @@
     <col min="8" max="8" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="2" spans="1:13" ht="21">
-      <c r="A2" s="1"/>
+    <row r="1" spans="2:13" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:13" ht="21">
       <c r="B2" s="66" t="s">
         <v>0</v>
       </c>
@@ -1364,7 +1362,7 @@
       <c r="D2" s="48"/>
       <c r="E2" s="6"/>
       <c r="F2" s="75" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G2" s="67"/>
       <c r="H2" s="67"/>
@@ -1374,8 +1372,7 @@
       <c r="L2" s="68"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" ht="21">
-      <c r="A3" s="1"/>
+    <row r="3" spans="2:13" ht="21">
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1391,10 +1388,9 @@
       <c r="L3" s="71"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" ht="21">
-      <c r="A4" s="1"/>
+    <row r="4" spans="2:13" ht="21">
       <c r="B4" s="64" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C4" s="65"/>
       <c r="D4" s="65"/>
@@ -1407,8 +1403,7 @@
       <c r="K4" s="70"/>
       <c r="L4" s="71"/>
     </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="1"/>
+    <row r="5" spans="2:13">
       <c r="B5" s="10"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -1421,8 +1416,7 @@
       <c r="K5" s="70"/>
       <c r="L5" s="71"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A6" s="1"/>
+    <row r="6" spans="2:13" ht="15.75" thickBot="1">
       <c r="B6" s="10"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -1435,8 +1429,7 @@
       <c r="K6" s="73"/>
       <c r="L6" s="74"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A7" s="1"/>
+    <row r="7" spans="2:13" ht="15.75" thickBot="1">
       <c r="B7" s="10"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -1450,8 +1443,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" ht="28.5">
-      <c r="A8" s="1"/>
+    <row r="8" spans="2:13" ht="28.5">
       <c r="B8" s="15" t="s">
         <v>2</v>
       </c>
@@ -1467,8 +1459,7 @@
       <c r="L8" s="18"/>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="1"/>
+    <row r="9" spans="2:13">
       <c r="B9" s="10"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -1481,8 +1472,7 @@
       <c r="K9" s="9"/>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="1"/>
+    <row r="10" spans="2:13">
       <c r="B10" s="10" t="s">
         <v>3</v>
       </c>
@@ -1499,8 +1489,7 @@
       <c r="K10" s="9"/>
       <c r="L10" s="11"/>
     </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="1"/>
+    <row r="11" spans="2:13">
       <c r="B11" s="10"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -1513,8 +1502,7 @@
       <c r="K11" s="9"/>
       <c r="L11" s="11"/>
     </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="1"/>
+    <row r="12" spans="2:13">
       <c r="B12" s="10" t="s">
         <v>5</v>
       </c>
@@ -1529,8 +1517,7 @@
       <c r="K12" s="9"/>
       <c r="L12" s="11"/>
     </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="1"/>
+    <row r="13" spans="2:13">
       <c r="B13" s="10"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -1543,8 +1530,7 @@
       <c r="K13" s="9"/>
       <c r="L13" s="11"/>
     </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="1"/>
+    <row r="14" spans="2:13">
       <c r="B14" s="10" t="s">
         <v>6</v>
       </c>
@@ -1559,8 +1545,7 @@
       <c r="K14" s="9"/>
       <c r="L14" s="47"/>
     </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="1"/>
+    <row r="15" spans="2:13">
       <c r="B15" s="10"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -1573,8 +1558,7 @@
       <c r="K15" s="9"/>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="1"/>
+    <row r="16" spans="2:13">
       <c r="B16" s="10" t="s">
         <v>7</v>
       </c>
@@ -1590,7 +1574,6 @@
       <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="1"/>
       <c r="B17" s="10"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1667,18 +1650,16 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="1"/>
-      <c r="B22" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
+      <c r="B22" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="77"/>
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
       <c r="L22" s="18"/>
@@ -1686,16 +1667,14 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="1"/>
-      <c r="B23" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
       <c r="L23" s="11"/>
@@ -1703,19 +1682,17 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="1"/>
-      <c r="B24" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
       <c r="J24" s="9"/>
       <c r="K24" s="76" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="L24" s="20"/>
       <c r="M24" s="3"/>
@@ -1775,7 +1752,7 @@
       <c r="F28" s="28"/>
       <c r="G28" s="9"/>
       <c r="H28" s="54" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I28" s="55"/>
       <c r="J28" s="55"/>
@@ -1792,7 +1769,7 @@
       <c r="F29" s="29"/>
       <c r="G29" s="30"/>
       <c r="H29" s="57" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I29" s="58"/>
       <c r="J29" s="58"/>
@@ -1854,7 +1831,7 @@
       <c r="F33" s="37"/>
       <c r="G33" s="9"/>
       <c r="H33" s="51" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I33" s="52"/>
       <c r="J33" s="52"/>
@@ -1865,7 +1842,7 @@
     <row r="34" spans="1:13" ht="15.75" thickTop="1">
       <c r="A34" s="1"/>
       <c r="B34" s="63" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C34" s="58"/>
       <c r="D34" s="9"/>
@@ -1882,17 +1859,17 @@
     <row r="35" spans="1:13">
       <c r="A35" s="1"/>
       <c r="B35" s="41" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C35" s="42" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D35" s="61" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E35" s="62"/>
       <c r="F35" s="38" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -1935,17 +1912,17 @@
     <row r="38" spans="1:13">
       <c r="A38" s="1"/>
       <c r="B38" s="44" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
       <c r="H38" s="26" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I38" s="24"/>
       <c r="J38" s="24"/>
@@ -1962,7 +1939,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
       <c r="H39" s="40" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
@@ -1979,7 +1956,7 @@
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I40" s="35"/>
       <c r="J40" s="35"/>
@@ -2010,7 +1987,7 @@
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
       <c r="H42" s="19" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I42" s="17"/>
       <c r="J42" s="17"/>
@@ -2026,7 +2003,7 @@
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
       <c r="H43" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
@@ -2042,7 +2019,7 @@
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="45" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
@@ -2058,7 +2035,7 @@
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
       <c r="H45" s="46" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I45" s="13"/>
       <c r="J45" s="13"/>
@@ -2067,7 +2044,7 @@
       <c r="M45" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="H33:L33"/>
@@ -2078,6 +2055,7 @@
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="F2:L6"/>
+    <mergeCell ref="B22:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>